<commit_message>
Adding municiaplity based abandoned land data changing LUC emissions to biomass removal and SOC, and adding GHG categories for that
</commit_message>
<xml_diff>
--- a/data/GHG.xlsx
+++ b/data/GHG.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\biofuel_location\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\biofuel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="4" r:id="rId1"/>
-    <sheet name="LUC" sheetId="7" r:id="rId2"/>
-    <sheet name="län mapping" sheetId="8" r:id="rId3"/>
-    <sheet name="feedstock" sheetId="1" r:id="rId4"/>
-    <sheet name="Hsu_conversion" sheetId="2" r:id="rId5"/>
-    <sheet name="newEC_conversion" sheetId="5" r:id="rId6"/>
-    <sheet name="fossils" sheetId="6" r:id="rId7"/>
-    <sheet name="transport" sheetId="3" r:id="rId8"/>
+    <sheet name="LUCaboveground" sheetId="7" r:id="rId2"/>
+    <sheet name="SOC" sheetId="9" r:id="rId3"/>
+    <sheet name="län mapping" sheetId="8" r:id="rId4"/>
+    <sheet name="feedstock" sheetId="1" r:id="rId5"/>
+    <sheet name="Hsu_conversion" sheetId="2" r:id="rId6"/>
+    <sheet name="newEC_conversion" sheetId="5" r:id="rId7"/>
+    <sheet name="fossils" sheetId="6" r:id="rId8"/>
+    <sheet name="transport" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="112">
   <si>
     <t>county</t>
   </si>
@@ -345,6 +346,30 @@
   </si>
   <si>
     <t xml:space="preserve"> 32,78 GJ per m3, 69,68 kg co2 per GJ: 2286,077 (new number in 2021)</t>
+  </si>
+  <si>
+    <t>LUCabovenat</t>
+  </si>
+  <si>
+    <t>LUCabovecrp</t>
+  </si>
+  <si>
+    <t>SOCcrp</t>
+  </si>
+  <si>
+    <t>SOCgrassland</t>
+  </si>
+  <si>
+    <t>LUC</t>
+  </si>
+  <si>
+    <t>SOC</t>
+  </si>
+  <si>
+    <t>grassland to perennial bioenergy grass</t>
+  </si>
+  <si>
+    <t>ALA cropland to perennial bioenergy grass</t>
   </si>
 </sst>
 </file>
@@ -719,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,14 +1746,14 @@
         <v>92</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C71" s="5" t="str">
-        <f>LUC!A2</f>
+        <f>LUCaboveground!A2</f>
         <v>SE01</v>
       </c>
       <c r="D71" s="5">
-        <f>LUC!G2</f>
+        <f>LUCaboveground!G2</f>
         <v>655</v>
       </c>
     </row>
@@ -1737,14 +1762,14 @@
         <v>92</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C72" s="5" t="str">
-        <f>LUC!A3</f>
+        <f>LUCaboveground!A3</f>
         <v>SE02</v>
       </c>
       <c r="D72" s="5">
-        <f>LUC!G3</f>
+        <f>LUCaboveground!G3</f>
         <v>518</v>
       </c>
     </row>
@@ -1753,14 +1778,14 @@
         <v>92</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C73" s="5" t="str">
-        <f>LUC!A4</f>
+        <f>LUCaboveground!A4</f>
         <v>SE04</v>
       </c>
       <c r="D73" s="5">
-        <f>LUC!G4</f>
+        <f>LUCaboveground!G4</f>
         <v>1042.5</v>
       </c>
     </row>
@@ -1769,14 +1794,14 @@
         <v>92</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C74" s="5" t="str">
-        <f>LUC!A5</f>
+        <f>LUCaboveground!A5</f>
         <v>SE06</v>
       </c>
       <c r="D74" s="5">
-        <f>LUC!G5</f>
+        <f>LUCaboveground!G5</f>
         <v>896.00000000000011</v>
       </c>
     </row>
@@ -1785,14 +1810,14 @@
         <v>92</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C75" s="5" t="str">
-        <f>LUC!A6</f>
+        <f>LUCaboveground!A6</f>
         <v>SE07</v>
       </c>
       <c r="D75" s="5">
-        <f>LUC!G6</f>
+        <f>LUCaboveground!G6</f>
         <v>941.49999999999989</v>
       </c>
     </row>
@@ -1801,14 +1826,14 @@
         <v>92</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C76" s="5" t="str">
-        <f>LUC!A7</f>
+        <f>LUCaboveground!A7</f>
         <v>SE08</v>
       </c>
       <c r="D76" s="5">
-        <f>LUC!G7</f>
+        <f>LUCaboveground!G7</f>
         <v>727.00000000000011</v>
       </c>
     </row>
@@ -1817,14 +1842,14 @@
         <v>92</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C77" s="5" t="str">
-        <f>LUC!A8</f>
+        <f>LUCaboveground!A8</f>
         <v>SE09</v>
       </c>
       <c r="D77" s="5">
-        <f>LUC!G8</f>
+        <f>LUCaboveground!G8</f>
         <v>584.00000000000011</v>
       </c>
     </row>
@@ -1833,14 +1858,14 @@
         <v>92</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C78" s="5" t="str">
-        <f>LUC!A9</f>
+        <f>LUCaboveground!A9</f>
         <v>SE0A</v>
       </c>
       <c r="D78" s="5">
-        <f>LUC!G9</f>
+        <f>LUCaboveground!G9</f>
         <v>875.5</v>
       </c>
     </row>
@@ -1849,14 +1874,14 @@
         <v>92</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C79" s="5" t="str">
-        <f>LUC!A2</f>
+        <f>LUCaboveground!A2</f>
         <v>SE01</v>
       </c>
       <c r="D79">
-        <f>LUC!J2</f>
+        <f>LUCaboveground!J2</f>
         <v>-626.5</v>
       </c>
     </row>
@@ -1865,14 +1890,14 @@
         <v>92</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C80" s="5" t="str">
-        <f>LUC!A3</f>
+        <f>LUCaboveground!A3</f>
         <v>SE02</v>
       </c>
       <c r="D80" s="5">
-        <f>LUC!J3</f>
+        <f>LUCaboveground!J3</f>
         <v>-495.5</v>
       </c>
     </row>
@@ -1881,14 +1906,14 @@
         <v>92</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C81" s="5" t="str">
-        <f>LUC!A4</f>
+        <f>LUCaboveground!A4</f>
         <v>SE04</v>
       </c>
       <c r="D81" s="5">
-        <f>LUC!J4</f>
+        <f>LUCaboveground!J4</f>
         <v>-997.49999999999989</v>
       </c>
     </row>
@@ -1897,14 +1922,14 @@
         <v>92</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C82" s="5" t="str">
-        <f>LUC!A5</f>
+        <f>LUCaboveground!A5</f>
         <v>SE06</v>
       </c>
       <c r="D82" s="5">
-        <f>LUC!J5</f>
+        <f>LUCaboveground!J5</f>
         <v>-857.49999999999989</v>
       </c>
     </row>
@@ -1913,14 +1938,14 @@
         <v>92</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C83" s="5" t="str">
-        <f>LUC!A6</f>
+        <f>LUCaboveground!A6</f>
         <v>SE07</v>
       </c>
       <c r="D83" s="5">
-        <f>LUC!J6</f>
+        <f>LUCaboveground!J6</f>
         <v>-901.50000000000011</v>
       </c>
     </row>
@@ -1929,14 +1954,14 @@
         <v>92</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C84" s="5" t="str">
-        <f>LUC!A7</f>
+        <f>LUCaboveground!A7</f>
         <v>SE08</v>
       </c>
       <c r="D84" s="5">
-        <f>LUC!J7</f>
+        <f>LUCaboveground!J7</f>
         <v>-695.00000000000011</v>
       </c>
     </row>
@@ -1945,14 +1970,14 @@
         <v>92</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C85" s="5" t="str">
-        <f>LUC!A8</f>
+        <f>LUCaboveground!A8</f>
         <v>SE09</v>
       </c>
       <c r="D85" s="5">
-        <f>LUC!J8</f>
+        <f>LUCaboveground!J8</f>
         <v>-558.5</v>
       </c>
     </row>
@@ -1961,15 +1986,45 @@
         <v>92</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C86" s="5" t="str">
-        <f>LUC!A9</f>
+        <f>LUCaboveground!A9</f>
         <v>SE0A</v>
       </c>
       <c r="D86" s="5">
-        <f>LUC!J9</f>
+        <f>LUCaboveground!J9</f>
         <v>-838.00000000000011</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B87" t="s">
+        <v>106</v>
+      </c>
+      <c r="C87" t="s">
+        <v>26</v>
+      </c>
+      <c r="D87">
+        <f>SOC!B2</f>
+        <v>-5100</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B88" t="s">
+        <v>107</v>
+      </c>
+      <c r="C88" t="s">
+        <v>26</v>
+      </c>
+      <c r="D88">
+        <f>SOC!B3</f>
+        <v>13600</v>
       </c>
     </row>
   </sheetData>
@@ -1982,7 +2037,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2336,6 +2391,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2">
+        <v>-5100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3">
+        <v>13600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
@@ -2591,7 +2688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
@@ -2788,7 +2885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -2931,7 +3028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2977,11 +3074,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
@@ -3115,7 +3212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>

<commit_message>
SOC was not allocated to municipalities: this is solved Adding value of GHG of alternative use adding reference in ghg.xlsx Adding scenarios
</commit_message>
<xml_diff>
--- a/data/GHG.xlsx
+++ b/data/GHG.xlsx
@@ -15,12 +15,13 @@
     <sheet name="all" sheetId="4" r:id="rId1"/>
     <sheet name="LUCaboveground" sheetId="7" r:id="rId2"/>
     <sheet name="SOC" sheetId="9" r:id="rId3"/>
-    <sheet name="län mapping" sheetId="8" r:id="rId4"/>
-    <sheet name="feedstock" sheetId="1" r:id="rId5"/>
-    <sheet name="Hsu_conversion" sheetId="2" r:id="rId6"/>
-    <sheet name="newEC_conversion" sheetId="5" r:id="rId7"/>
-    <sheet name="fossils" sheetId="6" r:id="rId8"/>
-    <sheet name="transport" sheetId="3" r:id="rId9"/>
+    <sheet name="alternative use" sheetId="10" r:id="rId4"/>
+    <sheet name="län mapping" sheetId="8" r:id="rId5"/>
+    <sheet name="feedstock" sheetId="1" r:id="rId6"/>
+    <sheet name="Hsu_conversion" sheetId="2" r:id="rId7"/>
+    <sheet name="newEC_conversion" sheetId="5" r:id="rId8"/>
+    <sheet name="fossils" sheetId="6" r:id="rId9"/>
+    <sheet name="transport" sheetId="3" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="122">
   <si>
     <t>county</t>
   </si>
@@ -370,13 +371,45 @@
   </si>
   <si>
     <t>ALA cropland to perennial bioenergy grass</t>
+  </si>
+  <si>
+    <t>Cristina-Maria Iordan,  BaptisteGiroux, Jan Sandstad  Næss , Xiangping Hu,  Otávio Cavalett, Francesco Cherubini (2023). Energy potentials, negative emissions, and spatially explicit environmental impacts of perennial grasses on abandoned cropland in Europe Environmental Impact Assessment Review. Volume 98, https://doi.org/10.1016/j.eiar.2022.106942</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iordan et al Table 2: reed canary grass rainfed (but based on same grass all of them), lifecycle co2eq change t per hectare and year: 2.4, per t drymatter: 0.223. SOC -5.1 +/-8.1 t/hectare. </t>
+  </si>
+  <si>
+    <t>Ledo, A., Smith, P., Zerihun, A., Whitaker, J., Vicente-Vicente, J.L., Qin, Z., McNamara, N.P., Zinn, Y.L., Llorente, M., Liebig, M., Kuhnert, M., Dondini, M., Don, A., Diaz-Pines, E., Datta, A., Bakka, H., Aguilera, E., Hillier, J., 2020. Changes in soil organic carbon under perennial crops. Global Change Biol. 26, 4158–4168. https://doi.org/10.1111/gcb.15120.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ledo et al 2020. TABLE 1. Mean values of SOC (soil organic carbon) stocks (Mg/ha) and standard error of the mean before and after conversion to perennial with land use change more than 20 years ago.
+SOC change, to perennial grass, GLOBAL, 0-100 cm depth, mg/ha-year. From annula crop land: 5.7 +/-11 (11%). From grassland: -13.6 +/-8.9 (-9.6%). 
+</t>
+  </si>
+  <si>
+    <t>For comparisons, natural regrowth achieved a lower</t>
+  </si>
+  <si>
+    <t>average of 􀀀 5.9 ± 3.5 tCO2eq ha􀀀 1 year􀀀 1 on abandoned cropland</t>
+  </si>
+  <si>
+    <t>alternative use kg CO2 per hectare</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>altEmisALA</t>
+  </si>
+  <si>
+    <t>Næss, J. S., Hu, X., Gvein, M. H., Iordan, C. M., Cavalett, O., Dorber, M., ... &amp; Cherubini, F. (2023). Climate change mitigation potentials of biofuels produced from perennial crops and natural regrowth on abandoned and degraded cropland in Nordic countries. Journal of Environmental Management, 325, 116474. https://doi.org/10.1016/j.jenvman.2022.116474</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,6 +420,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -399,6 +433,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -427,11 +469,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -463,8 +506,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlänk" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -744,10 +794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2008,7 +2058,7 @@
         <v>26</v>
       </c>
       <c r="D87">
-        <f>SOC!B2</f>
+        <f>SOC!B3</f>
         <v>-5100</v>
       </c>
     </row>
@@ -2023,8 +2073,58 @@
         <v>26</v>
       </c>
       <c r="D88">
-        <f>SOC!B3</f>
+        <f>SOC!B4</f>
         <v>13600</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B89" t="s">
+        <v>120</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D89">
+        <f>'alternative use'!B5</f>
+        <v>5900</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="B2">
+        <f>A2*(0.12/0.153)</f>
+        <v>3.7647058823529415E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2391,10 +2491,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2402,36 +2502,98 @@
     <col min="1" max="1" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>108</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>111</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>-5100</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>110</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>13600</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="https://doi.org/10.1016/j.eiar.2022.106942"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5">
+        <v>5900</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://doi.org/10.1016/j.jenvman.2022.116474"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
@@ -2688,7 +2850,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
@@ -2885,7 +3047,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -3028,7 +3190,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -3074,7 +3236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
@@ -3210,39 +3372,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="B2">
-        <f>A2*(0.12/0.153)</f>
-        <v>3.7647058823529415E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>